<commit_message>
update plan and document
</commit_message>
<xml_diff>
--- a/Week 9/ProductBacklog-Version-1.0-1.xlsx
+++ b/Week 9/ProductBacklog-Version-1.0-1.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JavaWeb\swp391-onlineshop-gr1\Week 9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\KÌ 5 - SWP391 - G1\project\swp391-onlineshop-gr1\Week 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C5A5F0-3E36-4061-9FB8-DFE6E72261ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="109">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC (SWP391)</t>
   </si>
@@ -286,9 +298,6 @@
     <t>User Authoriation for system</t>
   </si>
   <si>
-    <t xml:space="preserve">Shipping </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Trần Văn Đức</t>
   </si>
   <si>
@@ -304,9 +313,6 @@
     <t>Customer views Feedback, edits  feedback of product</t>
   </si>
   <si>
-    <t>Project Work Item</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -322,9 +328,6 @@
     <t>Recording Link</t>
   </si>
   <si>
-    <t>Skills Training</t>
-  </si>
-  <si>
     <t>14h30 - 16h (15/09/2021)</t>
   </si>
   <si>
@@ -337,9 +340,6 @@
     <t>Link Record</t>
   </si>
   <si>
-    <t>Continue update SRS documents</t>
-  </si>
-  <si>
     <t>13/09/2021-17/09/2021</t>
   </si>
   <si>
@@ -349,37 +349,37 @@
     <t>All member</t>
   </si>
   <si>
-    <t>Skills Trainning</t>
-  </si>
-  <si>
     <t>21h-22h30(16/09/2021)</t>
   </si>
   <si>
     <t>JSP + servlet</t>
   </si>
   <si>
-    <t>Github</t>
-  </si>
-  <si>
     <t>21h-22h30(17/09/2021)</t>
   </si>
   <si>
     <t>Systax</t>
   </si>
   <si>
-    <t>JavaScript</t>
-  </si>
-  <si>
     <t>20h30-9h30(27/09/2021</t>
   </si>
   <si>
     <t>Syntax</t>
+  </si>
+  <si>
+    <t>Manager banner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK can manager banner and customer can view bannẻ </t>
+  </si>
+  <si>
+    <t>Ship-work</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="30">
     <font>
       <sz val="12"/>
@@ -652,7 +652,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -690,30 +690,39 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -721,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -829,32 +838,17 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -887,6 +881,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,7 +932,13 @@
     <xdr:ext cx="6734175" cy="762000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.png" descr="2017-FPTU-L-01"/>
+        <xdr:cNvPr id="2" name="image1.png" descr="2017-FPTU-L-01">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1134,27 +1156,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="44.125" customWidth="1"/>
-    <col min="4" max="4" width="25.25" customWidth="1"/>
-    <col min="5" max="5" width="18.875" customWidth="1"/>
-    <col min="6" max="6" width="22.25" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
+    <col min="3" max="3" width="44.09765625" customWidth="1"/>
+    <col min="4" max="4" width="25.19921875" customWidth="1"/>
+    <col min="5" max="5" width="18.8984375" customWidth="1"/>
+    <col min="6" max="6" width="22.19921875" customWidth="1"/>
+    <col min="7" max="7" width="16.09765625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:11" ht="15.6">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1163,10 +1185,10 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75">
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1175,10 +1197,10 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75">
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.6">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1187,10 +1209,10 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75">
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.6">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1199,10 +1221,10 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-    </row>
-    <row r="5" spans="1:11" ht="19.5">
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+    </row>
+    <row r="5" spans="1:11" ht="19.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1213,10 +1235,10 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75">
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1227,10 +1249,10 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.75">
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+    </row>
+    <row r="7" spans="1:11" ht="17.399999999999999">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="7"/>
@@ -1239,10 +1261,10 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-    </row>
-    <row r="8" spans="1:11" ht="18.75">
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+    </row>
+    <row r="8" spans="1:11" ht="18">
       <c r="A8" s="8" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1278,7 @@
       <c r="I8" s="15"/>
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75">
+    <row r="9" spans="1:11" ht="15.6">
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
@@ -1281,10 +1303,10 @@
       <c r="H9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="I9" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="49" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1311,11 +1333,11 @@
         <v>17</v>
       </c>
       <c r="H10" s="28"/>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="52">
-        <f t="shared" ref="J10:J40" si="0">IF(I10="Complex", 240, IF(I10="Medium",120,60))</f>
+      <c r="J10" s="47">
+        <f t="shared" ref="J10:J41" si="0">IF(I10="Complex", 240, IF(I10="Medium",120,60))</f>
         <v>120</v>
       </c>
     </row>
@@ -1342,10 +1364,10 @@
         <v>17</v>
       </c>
       <c r="H11" s="28"/>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="52">
+      <c r="J11" s="47">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
@@ -1373,10 +1395,10 @@
         <v>26</v>
       </c>
       <c r="H12" s="28"/>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="52">
+      <c r="J12" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -1404,10 +1426,10 @@
         <v>17</v>
       </c>
       <c r="H13" s="28"/>
-      <c r="I13" s="56" t="s">
+      <c r="I13" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="52">
+      <c r="J13" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -1435,14 +1457,14 @@
         <v>17</v>
       </c>
       <c r="H14" s="28"/>
-      <c r="I14" s="56" t="s">
+      <c r="I14" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="52">
+      <c r="J14" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="K14" s="58"/>
+      <c r="K14" s="53"/>
     </row>
     <row r="15" spans="1:11" ht="39.75" customHeight="1">
       <c r="A15" s="21">
@@ -1467,10 +1489,10 @@
         <v>17</v>
       </c>
       <c r="H15" s="28"/>
-      <c r="I15" s="56" t="s">
+      <c r="I15" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="52">
+      <c r="J15" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1498,10 +1520,10 @@
         <v>17</v>
       </c>
       <c r="H16" s="28"/>
-      <c r="I16" s="56" t="s">
+      <c r="I16" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="52">
+      <c r="J16" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -1529,10 +1551,10 @@
         <v>41</v>
       </c>
       <c r="H17" s="28"/>
-      <c r="I17" s="56" t="s">
+      <c r="I17" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="52">
+      <c r="J17" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1560,10 +1582,10 @@
         <v>17</v>
       </c>
       <c r="H18" s="28"/>
-      <c r="I18" s="56" t="s">
+      <c r="I18" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="52">
+      <c r="J18" s="47">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
@@ -1591,10 +1613,10 @@
         <v>17</v>
       </c>
       <c r="H19" s="28"/>
-      <c r="I19" s="56" t="s">
+      <c r="I19" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="52">
+      <c r="J19" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -1622,10 +1644,10 @@
         <v>17</v>
       </c>
       <c r="H20" s="28"/>
-      <c r="I20" s="55" t="s">
+      <c r="I20" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="52">
+      <c r="J20" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1653,10 +1675,10 @@
         <v>17</v>
       </c>
       <c r="H21" s="28"/>
-      <c r="I21" s="56" t="s">
+      <c r="I21" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="52">
+      <c r="J21" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1684,10 +1706,10 @@
         <v>17</v>
       </c>
       <c r="H22" s="28"/>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="52">
+      <c r="J22" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1715,10 +1737,10 @@
         <v>41</v>
       </c>
       <c r="H23" s="28"/>
-      <c r="I23" s="55" t="s">
+      <c r="I23" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="52">
+      <c r="J23" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -1746,10 +1768,10 @@
         <v>17</v>
       </c>
       <c r="H24" s="28"/>
-      <c r="I24" s="55" t="s">
+      <c r="I24" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="52">
+      <c r="J24" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -1777,10 +1799,10 @@
         <v>17</v>
       </c>
       <c r="H25" s="28"/>
-      <c r="I25" s="55" t="s">
+      <c r="I25" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J25" s="52">
+      <c r="J25" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1808,10 +1830,10 @@
         <v>41</v>
       </c>
       <c r="H26" s="28"/>
-      <c r="I26" s="56" t="s">
+      <c r="I26" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="52">
+      <c r="J26" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1839,10 +1861,10 @@
         <v>26</v>
       </c>
       <c r="H27" s="28"/>
-      <c r="I27" s="55" t="s">
+      <c r="I27" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="52">
+      <c r="J27" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1870,10 +1892,10 @@
         <v>17</v>
       </c>
       <c r="H28" s="28"/>
-      <c r="I28" s="56" t="s">
+      <c r="I28" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="52">
+      <c r="J28" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1901,10 +1923,10 @@
         <v>17</v>
       </c>
       <c r="H29" s="28"/>
-      <c r="I29" s="56" t="s">
+      <c r="I29" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="52">
+      <c r="J29" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1932,10 +1954,10 @@
         <v>17</v>
       </c>
       <c r="H30" s="28"/>
-      <c r="I30" s="55" t="s">
+      <c r="I30" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="52">
+      <c r="J30" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1963,10 +1985,10 @@
         <v>17</v>
       </c>
       <c r="H31" s="28"/>
-      <c r="I31" s="55" t="s">
+      <c r="I31" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="52">
+      <c r="J31" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1994,15 +2016,15 @@
         <v>17</v>
       </c>
       <c r="H32" s="37"/>
-      <c r="I32" s="55" t="s">
+      <c r="I32" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="52">
+      <c r="J32" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="45.75" customHeight="1">
+    <row r="33" spans="1:10" ht="45.75" customHeight="1">
       <c r="A33" s="36">
         <v>24</v>
       </c>
@@ -2025,15 +2047,15 @@
         <v>17</v>
       </c>
       <c r="H33" s="38"/>
-      <c r="I33" s="56" t="s">
+      <c r="I33" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J33" s="52">
+      <c r="J33" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="43.5" customHeight="1">
+    <row r="34" spans="1:10" ht="43.5" customHeight="1">
       <c r="A34" s="36">
         <v>25</v>
       </c>
@@ -2052,15 +2074,15 @@
         <v>41</v>
       </c>
       <c r="H34" s="38"/>
-      <c r="I34" s="56" t="s">
+      <c r="I34" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="52">
+      <c r="J34" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="39" customHeight="1">
+    <row r="35" spans="1:10" ht="39" customHeight="1">
       <c r="A35" s="36">
         <v>26</v>
       </c>
@@ -2079,15 +2101,15 @@
         <v>41</v>
       </c>
       <c r="H35" s="38"/>
-      <c r="I35" s="56" t="s">
+      <c r="I35" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="52">
+      <c r="J35" s="47">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="40.5" customHeight="1">
+    <row r="36" spans="1:10" ht="40.5" customHeight="1">
       <c r="A36" s="36">
         <v>27</v>
       </c>
@@ -2106,20 +2128,20 @@
         <v>41</v>
       </c>
       <c r="H36" s="38"/>
-      <c r="I36" s="56" t="s">
+      <c r="I36" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="52">
+      <c r="J36" s="47">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="44.25" customHeight="1">
+    <row r="37" spans="1:10" ht="44.25" customHeight="1">
       <c r="A37" s="36">
         <v>28</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="35"/>
@@ -2131,15 +2153,15 @@
         <v>41</v>
       </c>
       <c r="H37" s="38"/>
-      <c r="I37" s="56" t="s">
+      <c r="I37" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J37" s="52">
+      <c r="J37" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="51" customHeight="1">
+    <row r="38" spans="1:10" ht="51" customHeight="1">
       <c r="A38" s="21">
         <v>29</v>
       </c>
@@ -2156,29 +2178,29 @@
         <v>44506</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G38" s="27" t="s">
         <v>17</v>
       </c>
       <c r="H38" s="38"/>
-      <c r="I38" s="55" t="s">
+      <c r="I38" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="52">
+      <c r="J38" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="45">
+    <row r="39" spans="1:10" ht="45">
       <c r="A39" s="21">
         <v>30</v>
       </c>
       <c r="B39" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>85</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>86</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="33"/>
@@ -2189,23 +2211,23 @@
         <v>41</v>
       </c>
       <c r="H39" s="38"/>
-      <c r="I39" s="55" t="s">
+      <c r="I39" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J39" s="52">
+      <c r="J39" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="45">
+    <row r="40" spans="1:10" ht="45">
       <c r="A40" s="21">
         <v>31</v>
       </c>
       <c r="B40" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="23" t="s">
         <v>87</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>88</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="33"/>
@@ -2216,242 +2238,180 @@
         <v>41</v>
       </c>
       <c r="H40" s="38"/>
-      <c r="I40" s="55" t="s">
+      <c r="I40" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J40" s="52">
+      <c r="J40" s="47">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="15.75">
-      <c r="I41" s="39"/>
-      <c r="J41" s="57"/>
-    </row>
-    <row r="42" spans="1:22" ht="26.25">
-      <c r="A42" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="40" t="s">
+    <row r="41" spans="1:10" s="61" customFormat="1" ht="30">
+      <c r="A41" s="54">
+        <v>32</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="57"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" s="38"/>
+      <c r="I41" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="47">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.6">
+      <c r="I42" s="42"/>
+      <c r="J42" s="52"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.6">
+      <c r="I43" s="42"/>
+      <c r="J43" s="52"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.6">
+      <c r="I44" s="42"/>
+      <c r="J44" s="52"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.6">
+      <c r="I45" s="42"/>
+      <c r="J45" s="52"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.6">
+      <c r="I46" s="42"/>
+      <c r="J46" s="52"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.6">
+      <c r="I47" s="42"/>
+      <c r="J47" s="52"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.6">
+      <c r="I48" s="42"/>
+      <c r="J48" s="52"/>
+    </row>
+    <row r="58" spans="1:5" ht="15" customHeight="1">
+      <c r="A58" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C58" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D58" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E58" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="40" t="s">
+    </row>
+    <row r="59" spans="1:5" ht="15" customHeight="1">
+      <c r="A59" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="G42" s="40" t="s">
+      <c r="B59" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="57"/>
-    </row>
-    <row r="43" spans="1:22" ht="15.75">
-      <c r="A43" s="41">
-        <v>1</v>
-      </c>
-      <c r="B43" s="42" t="s">
+      <c r="C59" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="42" t="s">
+      <c r="D59" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="42" t="s">
+    </row>
+    <row r="60" spans="1:5" ht="15" customHeight="1">
+      <c r="A60" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E43" s="43" t="s">
+      <c r="B60" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="43" t="s">
+      <c r="C60" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D60" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="H43" s="44"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="57"/>
-      <c r="K43" s="46"/>
-      <c r="L43" s="46"/>
-      <c r="M43" s="46"/>
-      <c r="N43" s="46"/>
-      <c r="O43" s="46"/>
-      <c r="P43" s="46"/>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="46"/>
-      <c r="S43" s="46"/>
-      <c r="T43" s="46"/>
-      <c r="U43" s="46"/>
-      <c r="V43" s="46"/>
-    </row>
-    <row r="44" spans="1:22" ht="26.25">
-      <c r="A44" s="47">
-        <v>2</v>
-      </c>
-      <c r="B44" s="48" t="s">
+      <c r="E60" s="45"/>
+    </row>
+    <row r="61" spans="1:5" ht="15" customHeight="1">
+      <c r="A61" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="48" t="s">
+      <c r="B61" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="48" t="s">
+      <c r="C61" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" customHeight="1">
+      <c r="A62" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="E44" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F44" s="48" t="s">
+      <c r="B62" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="G44" s="50"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="46"/>
-      <c r="N44" s="46"/>
-      <c r="O44" s="46"/>
-      <c r="P44" s="46"/>
-      <c r="Q44" s="46"/>
-      <c r="R44" s="46"/>
-      <c r="S44" s="46"/>
-      <c r="T44" s="46"/>
-      <c r="U44" s="46"/>
-      <c r="V44" s="46"/>
-    </row>
-    <row r="45" spans="1:22" ht="15.75">
-      <c r="A45" s="41">
-        <v>3</v>
-      </c>
-      <c r="B45" s="42" t="s">
+      <c r="C62" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1">
+      <c r="A63" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="B63" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="E45" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" s="42" t="s">
+      <c r="C63" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="H45" s="44"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
-      <c r="N45" s="46"/>
-      <c r="O45" s="46"/>
-      <c r="P45" s="46"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="46"/>
-      <c r="S45" s="46"/>
-      <c r="T45" s="46"/>
-      <c r="U45" s="46"/>
-      <c r="V45" s="46"/>
-    </row>
-    <row r="46" spans="1:22" ht="15.75">
-      <c r="A46" s="47">
-        <v>4</v>
-      </c>
-      <c r="B46" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="48" t="s">
-        <v>109</v>
-      </c>
-      <c r="E46" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="H46" s="44"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="46"/>
-      <c r="N46" s="46"/>
-      <c r="O46" s="46"/>
-      <c r="P46" s="46"/>
-      <c r="Q46" s="46"/>
-      <c r="R46" s="46"/>
-      <c r="S46" s="46"/>
-      <c r="T46" s="46"/>
-      <c r="U46" s="46"/>
-      <c r="V46" s="46"/>
-    </row>
-    <row r="47" spans="1:22" ht="15.75">
-      <c r="A47" s="41">
-        <v>5</v>
-      </c>
-      <c r="B47" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="E47" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G47" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="H47" s="44"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="46"/>
-      <c r="N47" s="46"/>
-      <c r="O47" s="46"/>
-      <c r="P47" s="46"/>
-      <c r="Q47" s="46"/>
-      <c r="R47" s="46"/>
-      <c r="S47" s="46"/>
-      <c r="T47" s="46"/>
-      <c r="U47" s="46"/>
-      <c r="V47" s="46"/>
+      <c r="E63" s="41" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E43" r:id="rId1"/>
-    <hyperlink ref="G43" r:id="rId2"/>
-    <hyperlink ref="E44" r:id="rId3"/>
-    <hyperlink ref="E45" r:id="rId4"/>
-    <hyperlink ref="G45" r:id="rId5"/>
-    <hyperlink ref="E46" r:id="rId6"/>
-    <hyperlink ref="G46" r:id="rId7"/>
-    <hyperlink ref="E47" r:id="rId8"/>
-    <hyperlink ref="G47" r:id="rId9"/>
+    <hyperlink ref="E63" r:id="rId1" xr:uid="{E1501451-04A3-438F-87EF-7D3FBA0545FE}"/>
+    <hyperlink ref="C63" r:id="rId2" xr:uid="{82527237-111D-47B4-9FA4-CBD34F90D5F2}"/>
+    <hyperlink ref="E62" r:id="rId3" xr:uid="{A3E21FBD-3F97-4D6D-BF16-1B78FAA7374B}"/>
+    <hyperlink ref="C62" r:id="rId4" xr:uid="{37669A98-731A-4135-A35E-93F6DC67A5A8}"/>
+    <hyperlink ref="E61" r:id="rId5" xr:uid="{906F6CEF-FCAD-47F8-8341-0972EB1F5CAE}"/>
+    <hyperlink ref="C61" r:id="rId6" xr:uid="{0303D210-A753-4FA8-8352-698ED2BD5283}"/>
+    <hyperlink ref="C60" r:id="rId7" xr:uid="{914E0B72-0146-4D39-B613-D85B030E5F30}"/>
+    <hyperlink ref="E59" r:id="rId8" xr:uid="{9F3EF831-1A6D-4784-A811-64639AFE1C3E}"/>
+    <hyperlink ref="C59" r:id="rId9" xr:uid="{4CFEEAE8-5A65-4472-AC8C-9AF6DD3C4365}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId10"/>

</xml_diff>

<commit_message>
update dashboard marketing and sql
</commit_message>
<xml_diff>
--- a/Week 9/ProductBacklog-Version-1.0-1.xlsx
+++ b/Week 9/ProductBacklog-Version-1.0-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\SWP\swp391-onlineshop-gr1\Week 9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\SWP\Final\swp391-onlineshop-gr1\Week 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF246AA2-CD1F-4FAF-A4CA-A973D863749F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58469ADC-2045-4E53-85EA-A54EE63F9746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -439,15 +439,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -656,7 +647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -684,13 +675,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -730,11 +714,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -756,142 +792,132 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="20" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="18" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="18" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,7 +1175,7 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -1174,8 +1200,8 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="1"/>
@@ -1186,8 +1212,8 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="1"/>
@@ -1198,8 +1224,8 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="1"/>
@@ -1210,8 +1236,8 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:11" ht="19.5">
       <c r="A5" s="1"/>
@@ -1224,8 +1250,8 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="1"/>
@@ -1238,8 +1264,8 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="18.75">
       <c r="A7" s="1"/>
@@ -1250,1231 +1276,1234 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:11" ht="18.75">
       <c r="A8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
     </row>
     <row r="9" spans="1:11" ht="15.75">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="51" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30">
-      <c r="A10" s="21">
+      <c r="A10" s="11">
         <v>1</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="15">
         <v>44476</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="48" t="s">
+      <c r="H10" s="41"/>
+      <c r="I10" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="45">
         <f t="shared" ref="J10:J42" si="0">IF(I10="Complex", 240, IF(I10="Medium",120,60))</f>
         <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30">
-      <c r="A11" s="21">
+      <c r="A11" s="11">
         <v>2</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="15">
         <v>44476</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="49" t="s">
+      <c r="H11" s="41"/>
+      <c r="I11" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="47">
+      <c r="J11" s="45">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="48.75" customHeight="1">
-      <c r="A12" s="21">
+      <c r="A12" s="11">
         <v>3</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="15">
         <v>44476</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="49" t="s">
+      <c r="H12" s="41"/>
+      <c r="I12" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="47">
+      <c r="J12" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="48.75" customHeight="1">
-      <c r="A13" s="21">
+      <c r="A13" s="11">
         <v>4</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="15">
         <v>44476</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="49" t="s">
+      <c r="H13" s="41"/>
+      <c r="I13" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="48.75" customHeight="1">
-      <c r="A14" s="21">
+      <c r="A14" s="11">
         <v>5</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="15">
         <v>44476</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="49" t="s">
+      <c r="H14" s="41"/>
+      <c r="I14" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="45">
         <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="48.75" customHeight="1">
-      <c r="A15" s="21">
+      <c r="A15" s="11">
         <v>6</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="15">
         <v>44476</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="49" t="s">
+      <c r="H15" s="41"/>
+      <c r="I15" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="45">
         <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="33" customHeight="1">
-      <c r="A16" s="21">
+      <c r="A16" s="11">
         <v>7</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="15">
         <v>44476</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="49" t="s">
+      <c r="H16" s="41"/>
+      <c r="I16" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="47">
+      <c r="J16" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="K16" s="51"/>
+      <c r="K16" s="35"/>
     </row>
     <row r="17" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A17" s="21">
+      <c r="A17" s="11">
         <v>8</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="15">
         <v>44476</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="49" t="s">
+      <c r="H17" s="41"/>
+      <c r="I17" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A18" s="21">
+      <c r="A18" s="11">
         <v>9</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="15">
         <v>44486</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="49" t="s">
+      <c r="H18" s="41"/>
+      <c r="I18" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A19" s="21">
+      <c r="A19" s="11">
         <v>10</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="15">
         <v>44486</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="49" t="s">
+      <c r="H19" s="41"/>
+      <c r="I19" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A20" s="21">
+      <c r="A20" s="11">
         <v>11</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="15">
         <v>44476</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="49" t="s">
+      <c r="H20" s="41"/>
+      <c r="I20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="47">
+      <c r="J20" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A21" s="21">
+      <c r="A21" s="11">
         <v>12</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="15">
         <v>44476</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="48" t="s">
+      <c r="H21" s="41"/>
+      <c r="I21" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="47">
+      <c r="J21" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A22" s="21">
+      <c r="A22" s="11">
         <v>13</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="15">
         <v>44476</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="49" t="s">
+      <c r="H22" s="41"/>
+      <c r="I22" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="47">
+      <c r="J22" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A23" s="21">
+      <c r="A23" s="11">
         <v>14</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="15">
         <v>44486</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="48" t="s">
+      <c r="H23" s="41"/>
+      <c r="I23" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J23" s="47">
+      <c r="J23" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="49.5" customHeight="1">
-      <c r="A24" s="21">
+      <c r="A24" s="11">
         <v>15</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="15">
         <v>44486</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="48" t="s">
+      <c r="H24" s="41"/>
+      <c r="I24" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="47">
+      <c r="J24" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A25" s="21">
+      <c r="A25" s="11">
         <v>16</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="15">
         <v>44486</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="48" t="s">
+      <c r="H25" s="41"/>
+      <c r="I25" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="47">
+      <c r="J25" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A26" s="21">
+      <c r="A26" s="11">
         <v>17</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="22">
         <v>44506</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="48" t="s">
+      <c r="H26" s="41"/>
+      <c r="I26" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="47">
+      <c r="J26" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A27" s="21">
+      <c r="A27" s="11">
         <v>18</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="22">
         <v>44506</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="49" t="s">
+      <c r="H27" s="41"/>
+      <c r="I27" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="47">
+      <c r="J27" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A28" s="21">
+      <c r="A28" s="11">
         <v>19</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="15">
         <v>44486</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="48" t="s">
+      <c r="H28" s="41"/>
+      <c r="I28" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="47">
+      <c r="J28" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A29" s="34">
+      <c r="A29" s="23">
         <v>20</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="15">
         <v>44476</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G29" s="27" t="s">
+      <c r="G29" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="49" t="s">
+      <c r="H29" s="41"/>
+      <c r="I29" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="47">
+      <c r="J29" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="48" customHeight="1">
-      <c r="A30" s="34">
+      <c r="A30" s="23">
         <v>21</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="15">
         <v>44476</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="28"/>
-      <c r="I30" s="49" t="s">
+      <c r="H30" s="41"/>
+      <c r="I30" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="47">
+      <c r="J30" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="48" customHeight="1">
-      <c r="A31" s="34">
+      <c r="A31" s="23">
         <v>22</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="33">
+      <c r="E31" s="22">
         <v>44506</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G31" s="27" t="s">
+      <c r="G31" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="48" t="s">
+      <c r="H31" s="41"/>
+      <c r="I31" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="47">
+      <c r="J31" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="44.25" customHeight="1">
-      <c r="A32" s="36">
+      <c r="A32" s="25">
         <v>23</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="22">
         <v>44506</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="G32" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="28"/>
-      <c r="I32" s="48" t="s">
+      <c r="H32" s="41"/>
+      <c r="I32" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="47">
+      <c r="J32" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A33" s="21">
+      <c r="A33" s="11">
         <v>24</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="33">
+      <c r="E33" s="22">
         <v>44506</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="48" t="s">
+      <c r="H33" s="42"/>
+      <c r="I33" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="47">
+      <c r="J33" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45.75" customHeight="1">
-      <c r="A34" s="36">
+      <c r="A34" s="25">
         <v>25</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="33">
+      <c r="E34" s="22">
         <v>44506</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="F34" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G34" s="27" t="s">
+      <c r="G34" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="38"/>
-      <c r="I34" s="49" t="s">
+      <c r="H34" s="43"/>
+      <c r="I34" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="47">
+      <c r="J34" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="43.5" customHeight="1">
-      <c r="A35" s="36">
+      <c r="A35" s="25">
         <v>26</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="33">
+      <c r="E35" s="22">
         <v>44506</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="F35" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="32" t="s">
+      <c r="G35" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H35" s="38"/>
-      <c r="I35" s="49" t="s">
+      <c r="H35" s="43"/>
+      <c r="I35" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="47">
+      <c r="J35" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="39" customHeight="1">
-      <c r="A36" s="36">
+      <c r="A36" s="25">
         <v>27</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="33">
+      <c r="E36" s="22">
         <v>44506</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G36" s="32" t="s">
+      <c r="G36" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="38"/>
-      <c r="I36" s="49" t="s">
+      <c r="H36" s="43"/>
+      <c r="I36" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="47">
+      <c r="J36" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A37" s="36">
+      <c r="A37" s="25">
         <v>28</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="33">
+      <c r="E37" s="22">
         <v>44506</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="27" t="s">
+      <c r="G37" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="38"/>
-      <c r="I37" s="49" t="s">
+      <c r="H37" s="43"/>
+      <c r="I37" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="47">
+      <c r="J37" s="45">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="44.25" customHeight="1">
-      <c r="A38" s="36">
+      <c r="A38" s="25">
         <v>29</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="24" t="s">
+      <c r="C38" s="19"/>
+      <c r="D38" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="33">
+      <c r="E38" s="22">
         <v>44506</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="32" t="s">
+      <c r="G38" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H38" s="38"/>
-      <c r="I38" s="49" t="s">
+      <c r="H38" s="43"/>
+      <c r="I38" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="47">
+      <c r="J38" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="51" customHeight="1">
-      <c r="A39" s="21">
+      <c r="A39" s="11">
         <v>30</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="24" t="s">
+      <c r="D39" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="33">
+      <c r="E39" s="22">
         <v>44506</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="27" t="s">
+      <c r="G39" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="38"/>
-      <c r="I39" s="48" t="s">
+      <c r="H39" s="43"/>
+      <c r="I39" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J39" s="47">
+      <c r="J39" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="45">
-      <c r="A40" s="21">
+      <c r="A40" s="11">
         <v>31</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D40" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="33">
+      <c r="E40" s="22">
         <v>44506</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G40" s="32" t="s">
+      <c r="G40" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H40" s="38"/>
-      <c r="I40" s="48" t="s">
+      <c r="H40" s="43"/>
+      <c r="I40" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J40" s="47">
+      <c r="J40" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="45">
-      <c r="A41" s="21">
+      <c r="A41" s="11">
         <v>32</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E41" s="33">
+      <c r="E41" s="22">
         <v>44506</v>
       </c>
-      <c r="F41" s="26" t="s">
+      <c r="F41" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G41" s="32" t="s">
+      <c r="G41" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H41" s="38"/>
-      <c r="I41" s="48" t="s">
+      <c r="H41" s="43"/>
+      <c r="I41" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="J41" s="47">
+      <c r="J41" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="56" customFormat="1" ht="30">
-      <c r="A42" s="52">
+    <row r="42" spans="1:10" s="40" customFormat="1" ht="30">
+      <c r="A42" s="36">
         <v>33</v>
       </c>
-      <c r="B42" s="53" t="s">
+      <c r="B42" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="24" t="s">
+      <c r="D42" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="33">
+      <c r="E42" s="22">
         <v>44506</v>
       </c>
-      <c r="F42" s="55" t="s">
+      <c r="F42" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="27" t="s">
+      <c r="G42" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="38"/>
-      <c r="I42" s="48" t="s">
+      <c r="H42" s="43"/>
+      <c r="I42" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="47">
+      <c r="J42" s="45">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30">
-      <c r="A43" s="52">
+      <c r="A43" s="36">
         <v>34</v>
       </c>
-      <c r="B43" s="53" t="s">
+      <c r="B43" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C43" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D43" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="33">
+      <c r="E43" s="22">
         <v>44506</v>
       </c>
-      <c r="F43" s="55" t="s">
+      <c r="F43" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G43" s="27" t="s">
+      <c r="G43" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H43" s="38"/>
-      <c r="I43" s="48" t="s">
+      <c r="H43" s="43"/>
+      <c r="I43" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J43" s="47">
+      <c r="J43" s="45">
         <f t="shared" ref="J43" si="1">IF(I43="Complex", 240, IF(I43="Medium",120,60))</f>
         <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75">
-      <c r="I44" s="42"/>
-      <c r="J44" s="50"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="I45" s="42"/>
-      <c r="J45" s="50"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="I46" s="42"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10" ht="15.75">
-      <c r="I47" s="42"/>
-      <c r="J47" s="50"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="34"/>
     </row>
     <row r="48" spans="1:10" ht="15.75">
-      <c r="I48" s="42"/>
-      <c r="J48" s="50"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="34"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="I49" s="42"/>
-      <c r="J49" s="50"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="34"/>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B59" s="39" t="s">
+      <c r="B59" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C59" s="39" t="s">
+      <c r="C59" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D59" s="39" t="s">
+      <c r="D59" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="E59" s="39" t="s">
+      <c r="E59" s="26" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1">
-      <c r="A60" s="40" t="s">
+      <c r="A60" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="40" t="s">
+      <c r="D60" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E60" s="41" t="s">
+      <c r="E60" s="28" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C61" s="44" t="s">
+      <c r="C61" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D61" s="43" t="s">
+      <c r="D61" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="E61" s="45"/>
+      <c r="E61" s="32"/>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="B62" s="40" t="s">
+      <c r="B62" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="D62" s="40" t="s">
+      <c r="D62" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="28" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C63" s="44" t="s">
+      <c r="C63" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D63" s="43" t="s">
+      <c r="D63" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E63" s="44" t="s">
+      <c r="E63" s="31" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="C64" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="D64" s="40" t="s">
+      <c r="D64" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E64" s="41" t="s">
+      <c r="E64" s="28" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C8:J8"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="E64" r:id="rId1" xr:uid="{E1501451-04A3-438F-87EF-7D3FBA0545FE}"/>
     <hyperlink ref="C64" r:id="rId2" xr:uid="{82527237-111D-47B4-9FA4-CBD34F90D5F2}"/>

</xml_diff>